<commit_message>
process geometry function has been implemented
</commit_message>
<xml_diff>
--- a/static/stability/components.xlsx
+++ b/static/stability/components.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zpos(m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ypos(m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xpos(m)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight(kg)</t>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mass</t>
   </si>
   <si>
     <t xml:space="preserve">Front bumper</t>
@@ -284,8 +284,8 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>